<commit_message>
Added data-driven user registration using Excel and implemented Cucumber steps for Register.feature
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit\NewEclipseWorkSpace\AutomationExerciseBDDFramework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9CBF787-F55C-4FC3-948D-0A53262E275A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6E8E07-7B9D-4E12-899A-2D2F7D2342FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{2A5EA84E-2B2B-4B79-A6A3-79B2EA0AF481}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{2A5EA84E-2B2B-4B79-A6A3-79B2EA0AF481}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RegisterData" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>ankitredhu12@gmail.com</t>
   </si>
@@ -60,13 +61,37 @@
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Aanu</t>
+  </si>
+  <si>
+    <t>ankitredhu1100@gmail.com</t>
+  </si>
+  <si>
+    <t>Ankit</t>
+  </si>
+  <si>
+    <t>ankitredhu2201@gmail.com</t>
+  </si>
+  <si>
+    <t>Sachin</t>
+  </si>
+  <si>
+    <t>Sachin123498@gmail.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +103,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -104,9 +137,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -444,7 +486,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{357DA99E-2CC6-403F-93B1-8F69F56C68E0}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -494,4 +536,75 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B064BF34-2486-4580-93DE-5974B3EE2987}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="21.42578125" customWidth="1"/>
+    <col min="3" max="3" width="21.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{0C1DA07F-6872-4D2D-92A9-2D70936177C2}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{57B0CDB1-0853-4BD0-8E1B-5443E6E10466}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{A4E0F294-5CFE-4F5F-BD63-41DBB4C201E8}"/>
+    <hyperlink ref="C3" r:id="rId4" xr:uid="{660E5FFB-AA4F-4A24-BC61-D891EDBD9A0E}"/>
+    <hyperlink ref="B4" r:id="rId5" xr:uid="{DA52CF2B-E251-4336-9159-64D1DE01E8D4}"/>
+    <hyperlink ref="C4" r:id="rId6" xr:uid="{8F14F1E8-5674-49BF-A594-5ED5B4F94AA0}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Implemented CheckoutPage with delivery address, order review, comment entry, and place order actions
</commit_message>
<xml_diff>
--- a/testdata/TestData.xlsx
+++ b/testdata/TestData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ankit\NewEclipseWorkSpace\AutomationExerciseBDDFramework\testdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C6E8E07-7B9D-4E12-899A-2D2F7D2342FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DA3D2AB-9003-4FF7-A9F7-BBA221374A63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="1" xr2:uid="{2A5EA84E-2B2B-4B79-A6A3-79B2EA0AF481}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" activeTab="2" xr2:uid="{2A5EA84E-2B2B-4B79-A6A3-79B2EA0AF481}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="RegisterData" sheetId="2" r:id="rId2"/>
+    <sheet name="cardDetails" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>ankitredhu12@gmail.com</t>
   </si>
@@ -85,6 +86,21 @@
   </si>
   <si>
     <t>Sachin123498@gmail.com</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>card number</t>
+  </si>
+  <si>
+    <t>CVS</t>
+  </si>
+  <si>
+    <t>MM</t>
+  </si>
+  <si>
+    <t>YY</t>
   </si>
 </sst>
 </file>
@@ -137,7 +153,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -149,6 +165,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -542,7 +559,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B064BF34-2486-4580-93DE-5974B3EE2987}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -607,4 +624,56 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B62F1381-9B8C-4044-B325-5B403A41DD9F}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="30.140625" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="5">
+        <v>9652178523256980</v>
+      </c>
+      <c r="C2">
+        <v>652</v>
+      </c>
+      <c r="D2">
+        <v>11</v>
+      </c>
+      <c r="E2">
+        <v>2030</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>